<commit_message>
Migration to Automation Org
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/AR.xlsx
+++ b/templates/AutomationOrg/AR.xlsx
@@ -8,18 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAA354C-3B6B-46C8-B047-3BF3A291D1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C657C1-DE5C-42E2-8DA8-5C12506D688B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26670" yWindow="2445" windowWidth="19875" windowHeight="7875" tabRatio="761" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="525" yWindow="0" windowWidth="18330" windowHeight="11385" tabRatio="761" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
-    <sheet name="AddLine" sheetId="2" r:id="rId2"/>
-    <sheet name="FirmAllLines" sheetId="3" r:id="rId3"/>
-    <sheet name="Allocate" sheetId="5" r:id="rId4"/>
-    <sheet name="PickPackShip" sheetId="13" r:id="rId5"/>
-    <sheet name="CreateInvoice" sheetId="18" r:id="rId6"/>
-    <sheet name="CashReceipt" sheetId="21" r:id="rId7"/>
+    <sheet name="AddHeader_ForeignCurr" sheetId="23" r:id="rId2"/>
+    <sheet name="AddLine" sheetId="2" r:id="rId3"/>
+    <sheet name="AddLine_ForeignCurr" sheetId="24" r:id="rId4"/>
+    <sheet name="FirmAllLines" sheetId="3" r:id="rId5"/>
+    <sheet name="Allocate" sheetId="5" r:id="rId6"/>
+    <sheet name="PickPackShip" sheetId="13" r:id="rId7"/>
+    <sheet name="CreateInvoice" sheetId="18" r:id="rId8"/>
+    <sheet name="CashReceipt" sheetId="21" r:id="rId9"/>
+    <sheet name="CashReceipt_ForeignCurr" sheetId="22" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="44">
   <si>
     <t>API Mode</t>
   </si>
@@ -163,13 +166,22 @@
   </si>
   <si>
     <t>a6B5f000000PqATEA0</t>
+  </si>
+  <si>
+    <t>BC-INR</t>
+  </si>
+  <si>
+    <t>SR-INR</t>
+  </si>
+  <si>
+    <t>a6B5f000000PqiX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +214,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -223,12 +241,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +531,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,12 +596,147 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D908F63-2316-4814-8934-7E6571A2EA9A}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>450</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2">
+        <v>450</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D019CD-FE6F-4CBE-BD43-E1AA757A2A0A}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E477E4AB-7195-46E9-AE4C-74460C3E66C8}">
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,7 +1005,280 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DBB80D-3005-41F8-86F4-7517B0EFE4BC}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>200</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>20</v>
+      </c>
+      <c r="M2">
+        <v>30</v>
+      </c>
+      <c r="N2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>40</v>
+      </c>
+      <c r="M3">
+        <v>30</v>
+      </c>
+      <c r="N3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>50</v>
+      </c>
+      <c r="N4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>80</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>20</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A014ED-6B4B-4C73-85E3-BCAF80680504}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -888,7 +1315,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA382408-0CA4-42C9-9A0F-02454DC598A0}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -931,7 +1358,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3AAA29-D8B0-49CC-98B1-95E06AACF704}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -971,7 +1398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2448C880-E0DE-4186-968F-5BE216A9193B}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1012,12 +1439,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C10D85-D20E-4C13-9DFC-4F2EB5FB623F}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
AR TCs updated for Document Number field change
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/AR.xlsx
+++ b/templates/AutomationOrg/AR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C657C1-DE5C-42E2-8DA8-5C12506D688B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A3BF52-1F8F-444E-8637-D80E4C3732E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="0" windowWidth="18330" windowHeight="11385" tabRatio="761" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22755" yWindow="5310" windowWidth="15375" windowHeight="7875" tabRatio="761" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="45">
   <si>
     <t>API Mode</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>a6B5f000000PqiX</t>
+  </si>
+  <si>
+    <t>DivisionNumber</t>
   </si>
 </sst>
 </file>
@@ -598,42 +601,46 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D908F63-2316-4814-8934-7E6571A2EA9A}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>41</v>
       </c>
@@ -643,16 +650,19 @@
       <c r="C2">
         <v>100</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>450</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1441,47 +1451,51 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C10D85-D20E-4C13-9DFC-4F2EB5FB623F}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1491,16 +1505,19 @@
       <c r="C2">
         <v>100</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>38</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>450</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated AR Test Cases and started SO TC development in RSTKLUI
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/AR.xlsx
+++ b/templates/AutomationOrg/AR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A3BF52-1F8F-444E-8637-D80E4C3732E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D485713B-01BF-413E-A971-D20F4B8662F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22755" yWindow="5310" windowWidth="15375" windowHeight="7875" tabRatio="761" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="46">
   <si>
     <t>API Mode</t>
   </si>
@@ -168,9 +168,6 @@
     <t>a6B5f000000PqATEA0</t>
   </si>
   <si>
-    <t>BC-INR</t>
-  </si>
-  <si>
     <t>SR-INR</t>
   </si>
   <si>
@@ -178,6 +175,12 @@
   </si>
   <si>
     <t>DivisionNumber</t>
+  </si>
+  <si>
+    <t>SB BOI</t>
+  </si>
+  <si>
+    <t>a6B5f000000PqiXEAS</t>
   </si>
 </sst>
 </file>
@@ -604,7 +607,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +625,7 @@
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
         <v>26</v>
@@ -642,7 +645,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B2">
         <v>450</v>
@@ -654,10 +657,10 @@
         <v>100</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2">
         <v>450</v>
@@ -726,7 +729,7 @@
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
         <v>32</v>
@@ -1095,7 +1098,7 @@
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
         <v>32</v>
@@ -1139,7 +1142,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>32</v>
@@ -1183,7 +1186,7 @@
         <v>30</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>32</v>
@@ -1227,7 +1230,7 @@
         <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
         <v>32</v>
@@ -1262,7 +1265,7 @@
         <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
         <v>32</v>
@@ -1477,7 +1480,7 @@
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Updated AR excel file for Automation org
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/AR.xlsx
+++ b/templates/AutomationOrg/AR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D485713B-01BF-413E-A971-D20F4B8662F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0AFF66-6DD7-4D20-B07E-F328F0273F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="CreateInvoice" sheetId="18" r:id="rId8"/>
     <sheet name="CashReceipt" sheetId="21" r:id="rId9"/>
     <sheet name="CashReceipt_ForeignCurr" sheetId="22" r:id="rId10"/>
+    <sheet name="ARATO" sheetId="25" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="79">
   <si>
     <t>API Mode</t>
   </si>
@@ -175,6 +176,105 @@
   </si>
   <si>
     <t>DivisionNumber</t>
+  </si>
+  <si>
+    <t>FinancialDivision</t>
+  </si>
+  <si>
+    <t>FinancialCompany</t>
+  </si>
+  <si>
+    <t>Upload As Posted</t>
+  </si>
+  <si>
+    <t>Transaction Amount  AR Currency</t>
+  </si>
+  <si>
+    <t>Rate of Exchange</t>
+  </si>
+  <si>
+    <t>Credit Amount</t>
+  </si>
+  <si>
+    <t>Debit Amount</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Posting Type</t>
+  </si>
+  <si>
+    <t>Dimension Value 1</t>
+  </si>
+  <si>
+    <t>Dimension Value 2</t>
+  </si>
+  <si>
+    <t>Dimension Value 3</t>
+  </si>
+  <si>
+    <t>Dimension Value 4</t>
+  </si>
+  <si>
+    <t>Session Status</t>
+  </si>
+  <si>
+    <t>Current Value Transaction Currency</t>
+  </si>
+  <si>
+    <t>Current Value Home Currency</t>
+  </si>
+  <si>
+    <t>ExpectedGLTXNCount</t>
+  </si>
+  <si>
+    <t>a5B41000000PRNXEA4</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>a9h4100000005tC</t>
+  </si>
+  <si>
+    <t>a9g410000004LBs</t>
+  </si>
+  <si>
+    <t>a9S41000000Gnq3</t>
+  </si>
+  <si>
+    <t>Red Widgets</t>
+  </si>
+  <si>
+    <t>DIV11</t>
+  </si>
+  <si>
+    <t>TEST3</t>
+  </si>
+  <si>
+    <t>Green Widgets</t>
+  </si>
+  <si>
+    <t>Posted</t>
+  </si>
+  <si>
+    <t>Debit Memo</t>
+  </si>
+  <si>
+    <t>Credit Memo</t>
+  </si>
+  <si>
+    <t>a9S41000000GntC</t>
+  </si>
+  <si>
+    <t>Unapplied Cash</t>
+  </si>
+  <si>
+    <t>a5B410000004My9EAE</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
   <si>
     <t>SB BOI</t>
@@ -187,7 +287,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,12 +320,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF202124"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -247,13 +341,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,8 +737,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>44</v>
+      <c r="A2" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="B2">
         <v>450</v>
@@ -657,7 +750,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
         <v>41</v>
@@ -667,6 +760,977 @@
       </c>
       <c r="H2" t="s">
         <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3114FEA7-B434-48B1-B4F6-7B4F3BE8673D}">
+  <dimension ref="A1:S17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>500</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>500</v>
+      </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2">
+        <v>651</v>
+      </c>
+      <c r="L2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2">
+        <v>500</v>
+      </c>
+      <c r="R2">
+        <v>500</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>500</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>500</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3">
+        <v>601</v>
+      </c>
+      <c r="L3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M3" t="s">
+        <v>67</v>
+      </c>
+      <c r="N3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P3" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q3">
+        <v>500</v>
+      </c>
+      <c r="R3">
+        <v>500</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>500</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>500</v>
+      </c>
+      <c r="J4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4">
+        <v>611</v>
+      </c>
+      <c r="L4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q4">
+        <v>-500</v>
+      </c>
+      <c r="R4">
+        <v>-500</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>500</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>500</v>
+      </c>
+      <c r="J5" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5">
+        <v>613</v>
+      </c>
+      <c r="L5" t="s">
+        <v>66</v>
+      </c>
+      <c r="M5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N5" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" t="s">
+        <v>69</v>
+      </c>
+      <c r="P5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q5">
+        <v>-500</v>
+      </c>
+      <c r="R5">
+        <v>-500</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>500</v>
+      </c>
+      <c r="J6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6">
+        <v>651</v>
+      </c>
+      <c r="L6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N6" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" t="s">
+        <v>69</v>
+      </c>
+      <c r="P6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q6">
+        <v>50</v>
+      </c>
+      <c r="R6">
+        <v>500</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>500</v>
+      </c>
+      <c r="J7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K7">
+        <v>601</v>
+      </c>
+      <c r="L7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" t="s">
+        <v>68</v>
+      </c>
+      <c r="O7" t="s">
+        <v>69</v>
+      </c>
+      <c r="P7" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q7">
+        <v>50</v>
+      </c>
+      <c r="R7">
+        <v>500</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>500</v>
+      </c>
+      <c r="J8" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8">
+        <v>611</v>
+      </c>
+      <c r="L8" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N8" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" t="s">
+        <v>69</v>
+      </c>
+      <c r="P8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q8">
+        <v>-50</v>
+      </c>
+      <c r="R8">
+        <v>-500</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>500</v>
+      </c>
+      <c r="J9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9">
+        <v>613</v>
+      </c>
+      <c r="L9" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" t="s">
+        <v>67</v>
+      </c>
+      <c r="N9" t="s">
+        <v>68</v>
+      </c>
+      <c r="O9" t="s">
+        <v>69</v>
+      </c>
+      <c r="P9" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q9">
+        <v>-50</v>
+      </c>
+      <c r="R9">
+        <v>-500</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>500</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>500</v>
+      </c>
+      <c r="J10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10">
+        <v>651</v>
+      </c>
+      <c r="L10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N10" t="s">
+        <v>68</v>
+      </c>
+      <c r="O10" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q10">
+        <v>500</v>
+      </c>
+      <c r="R10">
+        <v>500</v>
+      </c>
+      <c r="S10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>500</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>500</v>
+      </c>
+      <c r="J11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11">
+        <v>601</v>
+      </c>
+      <c r="L11" t="s">
+        <v>66</v>
+      </c>
+      <c r="M11" t="s">
+        <v>67</v>
+      </c>
+      <c r="N11" t="s">
+        <v>68</v>
+      </c>
+      <c r="O11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q11">
+        <v>500</v>
+      </c>
+      <c r="R11">
+        <v>500</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>500</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>500</v>
+      </c>
+      <c r="J12" t="s">
+        <v>73</v>
+      </c>
+      <c r="K12">
+        <v>611</v>
+      </c>
+      <c r="L12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" t="s">
+        <v>67</v>
+      </c>
+      <c r="N12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O12" t="s">
+        <v>69</v>
+      </c>
+      <c r="P12" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q12">
+        <v>-500</v>
+      </c>
+      <c r="R12">
+        <v>-500</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>500</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>500</v>
+      </c>
+      <c r="J13" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13">
+        <v>613</v>
+      </c>
+      <c r="L13" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" t="s">
+        <v>67</v>
+      </c>
+      <c r="N13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O13" t="s">
+        <v>69</v>
+      </c>
+      <c r="P13" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q13">
+        <v>-500</v>
+      </c>
+      <c r="R13">
+        <v>-500</v>
+      </c>
+      <c r="S13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>50</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>500</v>
+      </c>
+      <c r="J14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14">
+        <v>651</v>
+      </c>
+      <c r="L14" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" t="s">
+        <v>67</v>
+      </c>
+      <c r="N14" t="s">
+        <v>68</v>
+      </c>
+      <c r="O14" t="s">
+        <v>69</v>
+      </c>
+      <c r="P14" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q14">
+        <v>50</v>
+      </c>
+      <c r="R14">
+        <v>500</v>
+      </c>
+      <c r="S14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>50</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>500</v>
+      </c>
+      <c r="J15" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15">
+        <v>601</v>
+      </c>
+      <c r="L15" t="s">
+        <v>66</v>
+      </c>
+      <c r="M15" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15" t="s">
+        <v>68</v>
+      </c>
+      <c r="O15" t="s">
+        <v>69</v>
+      </c>
+      <c r="P15" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q15">
+        <v>50</v>
+      </c>
+      <c r="R15">
+        <v>500</v>
+      </c>
+      <c r="S15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <v>500</v>
+      </c>
+      <c r="J16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K16">
+        <v>611</v>
+      </c>
+      <c r="L16" t="s">
+        <v>66</v>
+      </c>
+      <c r="M16" t="s">
+        <v>67</v>
+      </c>
+      <c r="N16" t="s">
+        <v>68</v>
+      </c>
+      <c r="O16" t="s">
+        <v>69</v>
+      </c>
+      <c r="P16" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q16">
+        <v>-50</v>
+      </c>
+      <c r="R16">
+        <v>-500</v>
+      </c>
+      <c r="S16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>50</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>500</v>
+      </c>
+      <c r="J17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K17">
+        <v>613</v>
+      </c>
+      <c r="L17" t="s">
+        <v>66</v>
+      </c>
+      <c r="M17" t="s">
+        <v>67</v>
+      </c>
+      <c r="N17" t="s">
+        <v>68</v>
+      </c>
+      <c r="O17" t="s">
+        <v>69</v>
+      </c>
+      <c r="P17" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q17">
+        <v>-50</v>
+      </c>
+      <c r="R17">
+        <v>-500</v>
+      </c>
+      <c r="S17">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test plan and AR TC through API
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/AR.xlsx
+++ b/templates/AutomationOrg/AR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\AutomationOrg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0AFF66-6DD7-4D20-B07E-F328F0273F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4B46FF-A484-4167-9F1D-99E6A38D502A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,14 @@
     <sheet name="AddLine" sheetId="2" r:id="rId3"/>
     <sheet name="AddLine_ForeignCurr" sheetId="24" r:id="rId4"/>
     <sheet name="FirmAllLines" sheetId="3" r:id="rId5"/>
-    <sheet name="Allocate" sheetId="5" r:id="rId6"/>
-    <sheet name="PickPackShip" sheetId="13" r:id="rId7"/>
-    <sheet name="CreateInvoice" sheetId="18" r:id="rId8"/>
-    <sheet name="CashReceipt" sheetId="21" r:id="rId9"/>
-    <sheet name="CashReceipt_ForeignCurr" sheetId="22" r:id="rId10"/>
-    <sheet name="ARATO" sheetId="25" r:id="rId11"/>
+    <sheet name="ApproveInvoice" sheetId="26" r:id="rId6"/>
+    <sheet name="TransferInvoice" sheetId="27" r:id="rId7"/>
+    <sheet name="Allocate" sheetId="5" r:id="rId8"/>
+    <sheet name="PickPackShip" sheetId="13" r:id="rId9"/>
+    <sheet name="CreateInvoice" sheetId="18" r:id="rId10"/>
+    <sheet name="CashReceipt" sheetId="21" r:id="rId11"/>
+    <sheet name="CashReceipt_ForeignCurr" sheetId="22" r:id="rId12"/>
+    <sheet name="ARATO" sheetId="25" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="81">
   <si>
     <t>API Mode</t>
   </si>
@@ -281,6 +283,12 @@
   </si>
   <si>
     <t>a6B5f000000PqiXEAS</t>
+  </si>
+  <si>
+    <t>Approve Sales Invoice</t>
+  </si>
+  <si>
+    <t>Transfer Sales Invoice</t>
   </si>
 </sst>
 </file>
@@ -696,10 +704,129 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2448C880-E0DE-4186-968F-5BE216A9193B}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C10D85-D20E-4C13-9DFC-4F2EB5FB623F}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>450</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2">
+        <v>450</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D908F63-2316-4814-8934-7E6571A2EA9A}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -768,7 +895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3114FEA7-B434-48B1-B4F6-7B4F3BE8673D}">
   <dimension ref="A1:S17"/>
   <sheetViews>
@@ -2393,6 +2520,80 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC3DC161-15A2-491A-8D79-715BD0C68AAA}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF58CD5-46D2-4094-A4C4-64F9F4BD8F76}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA382408-0CA4-42C9-9A0F-02454DC598A0}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2435,7 +2636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3AAA29-D8B0-49CC-98B1-95E06AACF704}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2473,123 +2674,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2448C880-E0DE-4186-968F-5BE216A9193B}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C10D85-D20E-4C13-9DFC-4F2EB5FB623F}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2">
-        <v>450</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2">
-        <v>450</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Create AR test case through UI
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/AR.xlsx
+++ b/templates/AutomationOrg/AR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4B46FF-A484-4167-9F1D-99E6A38D502A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B188BF4A-80C9-48CE-BF5B-F39554CADD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="88">
   <si>
     <t>API Mode</t>
   </si>
@@ -289,6 +289,27 @@
   </si>
   <si>
     <t>Transfer Sales Invoice</t>
+  </si>
+  <si>
+    <t>CustomerName</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Automation5501-1 (Stock-Mfg-LotYesSerialYes)</t>
+  </si>
+  <si>
+    <t>Automation5501-2 (Mfg-LotYes)</t>
+  </si>
+  <si>
+    <t>Automation5501-3 (Kit)</t>
+  </si>
+  <si>
+    <t>Automation5501-4 (Service)</t>
+  </si>
+  <si>
+    <t>Automation5501-5 (Misc)</t>
   </si>
 </sst>
 </file>
@@ -635,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,11 +668,12 @@
     <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -668,13 +690,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -691,9 +716,12 @@
         <v>31</v>
       </c>
       <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" t="b">
+      <c r="H2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1867,10 +1895,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D019CD-FE6F-4CBE-BD43-E1AA757A2A0A}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,11 +1907,12 @@
     <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1900,13 +1929,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1922,10 +1954,13 @@
       <c r="E2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" t="b">
+      <c r="H2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1937,10 +1972,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E477E4AB-7195-46E9-AE4C-74460C3E66C8}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="H1" sqref="H1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1951,13 +1986,14 @@
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1980,28 +2016,31 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2023,29 +2062,32 @@
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H2">
-        <v>1</v>
+      <c r="H2" t="s">
+        <v>83</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>200</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <v>20</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>30</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2067,29 +2109,32 @@
       <c r="G3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3">
         <v>2</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>100</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2</v>
       </c>
-      <c r="K3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3">
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3">
         <v>40</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>30</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2111,29 +2156,32 @@
       <c r="G4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H4">
-        <v>1</v>
+      <c r="H4" t="s">
+        <v>85</v>
       </c>
       <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>50</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="K4" t="b">
-        <v>1</v>
-      </c>
-      <c r="L4">
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>20</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>50</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -2155,20 +2203,23 @@
       <c r="G5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5">
         <v>2</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>80</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>4</v>
       </c>
-      <c r="K5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -2190,16 +2241,19 @@
       <c r="G6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6">
         <v>3</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>20</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>5</v>
       </c>
-      <c r="K6" t="b">
+      <c r="L6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2211,10 +2265,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DBB80D-3005-41F8-86F4-7517B0EFE4BC}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,13 +2279,14 @@
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2254,28 +2309,31 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2297,29 +2355,32 @@
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H2">
-        <v>1</v>
+      <c r="H2" t="s">
+        <v>83</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>200</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <v>20</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>30</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2341,29 +2402,32 @@
       <c r="G3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3">
         <v>2</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>100</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2</v>
       </c>
-      <c r="K3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3">
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3">
         <v>40</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>30</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2385,29 +2449,32 @@
       <c r="G4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H4">
-        <v>1</v>
+      <c r="H4" t="s">
+        <v>85</v>
       </c>
       <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>50</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="K4" t="b">
-        <v>1</v>
-      </c>
-      <c r="L4">
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>20</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>50</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -2429,20 +2496,23 @@
       <c r="G5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5">
         <v>2</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>80</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>4</v>
       </c>
-      <c r="K5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -2464,16 +2534,19 @@
       <c r="G6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6">
         <v>3</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>20</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>5</v>
       </c>
-      <c r="K6" t="b">
+      <c r="L6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2560,7 +2633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF58CD5-46D2-4094-A4C4-64F9F4BD8F76}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated CRATO - All API
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/AR.xlsx
+++ b/templates/AutomationOrg/AR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0614B879-CCE1-463F-9957-6D592256C4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D89DF0-FEA2-4718-AF1A-5DF86429607C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25140" yWindow="2475" windowWidth="16995" windowHeight="7140" tabRatio="761" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="101">
   <si>
     <t>API Mode</t>
   </si>
@@ -314,9 +314,6 @@
     <t>Automation5501-5 (Misc)</t>
   </si>
   <si>
-    <t>ComapnyID</t>
-  </si>
-  <si>
     <t>aBb5f0000004JfX</t>
   </si>
   <si>
@@ -339,12 +336,6 @@
   </si>
   <si>
     <t>TransactionAmountMaintCurr</t>
-  </si>
-  <si>
-    <t>HomeCurrtoMaintCurrRate</t>
-  </si>
-  <si>
-    <t>TransactionCurrtoHomeRate</t>
   </si>
   <si>
     <t>Not Yet Processed</t>
@@ -828,7 +819,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H2"/>
+      <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +840,7 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>25</v>
@@ -861,7 +852,7 @@
         <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="G1" t="s">
         <v>39</v>
@@ -881,7 +872,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2">
         <v>450</v>
@@ -893,7 +884,7 @@
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>40</v>
@@ -916,10 +907,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2BC7194-6154-49CA-A8FF-099750D7B793}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,15 +921,15 @@
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
         <v>39</v>
@@ -947,62 +938,50 @@
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>95</v>
+      <c r="I1" t="s">
+        <v>26</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2">
         <v>450</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="J2">
         <v>9</v>
       </c>
-      <c r="K2">
+      <c r="I2">
         <v>100</v>
       </c>
-      <c r="L2" t="s">
+      <c r="J2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1014,10 +993,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE6E911-31A5-440C-882A-670D99BCCC80}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,20 +1006,18 @@
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
         <v>39</v>
@@ -1049,62 +1026,50 @@
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>95</v>
+      <c r="I1" t="s">
+        <v>26</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B2">
         <v>450</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>78</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="H2">
-        <v>10</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="J2">
         <v>9</v>
       </c>
-      <c r="K2">
+      <c r="I2">
         <v>100</v>
       </c>
-      <c r="L2" t="s">
+      <c r="J2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1116,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D908F63-2316-4814-8934-7E6571A2EA9A}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1094,7 @@
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1154,8 +1119,11 @@
       <c r="H1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
@@ -1179,6 +1147,9 @@
       </c>
       <c r="H2" t="s">
         <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes related to labor booking and CPQ issues|added Test Plan for System Setup Behalf of pragati|System Setup changes
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/AR.xlsx
+++ b/templates/AutomationOrg/AR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D89DF0-FEA2-4718-AF1A-5DF86429607C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B188BF4A-80C9-48CE-BF5B-F39554CADD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25140" yWindow="2475" windowWidth="16995" windowHeight="7140" tabRatio="761" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,8 @@
     <sheet name="PickPackShip" sheetId="13" r:id="rId9"/>
     <sheet name="CreateInvoice" sheetId="18" r:id="rId10"/>
     <sheet name="CashReceipt" sheetId="21" r:id="rId11"/>
-    <sheet name="CRATO_HomeCurrency" sheetId="28" r:id="rId12"/>
-    <sheet name="CRATO_ForeignCurrency" sheetId="29" r:id="rId13"/>
-    <sheet name="CashReceipt_ForeignCurr" sheetId="22" r:id="rId14"/>
-    <sheet name="ARATO" sheetId="25" r:id="rId15"/>
+    <sheet name="CashReceipt_ForeignCurr" sheetId="22" r:id="rId12"/>
+    <sheet name="ARATO" sheetId="25" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="88">
   <si>
     <t>API Mode</t>
   </si>
@@ -312,45 +310,6 @@
   </si>
   <si>
     <t>Automation5501-5 (Misc)</t>
-  </si>
-  <si>
-    <t>aBb5f0000004JfX</t>
-  </si>
-  <si>
-    <t>BankAccountID</t>
-  </si>
-  <si>
-    <t>aBT5f000000wmhn</t>
-  </si>
-  <si>
-    <t>Check Payment</t>
-  </si>
-  <si>
-    <t>Transaction Currency</t>
-  </si>
-  <si>
-    <t>a8S5f0000004MBb</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>TransactionAmountMaintCurr</t>
-  </si>
-  <si>
-    <t>Not Yet Processed</t>
-  </si>
-  <si>
-    <t>DiscountTakenMaint Curr</t>
-  </si>
-  <si>
-    <t>CompanyID</t>
-  </si>
-  <si>
-    <t>aBT5f000000wmm0</t>
-  </si>
-  <si>
-    <t>a8S5f0000004NwM</t>
   </si>
 </sst>
 </file>
@@ -411,13 +370,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,86 +774,73 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C10D85-D20E-4C13-9DFC-4F2EB5FB623F}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
-        <v>89</v>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
       <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>98</v>
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" t="s">
+      <c r="H1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>90</v>
+      <c r="B2">
+        <v>450</v>
       </c>
       <c r="C2">
-        <v>450</v>
+        <v>100</v>
       </c>
       <c r="D2">
         <v>100</v>
       </c>
-      <c r="E2">
-        <v>100</v>
+      <c r="E2" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="G2">
+        <v>450</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2">
-        <v>450</v>
-      </c>
-      <c r="J2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -906,185 +851,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2BC7194-6154-49CA-A8FF-099750D7B793}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D908F63-2316-4814-8934-7E6571A2EA9A}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2">
-        <v>450</v>
-      </c>
-      <c r="C2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="H2">
-        <v>9</v>
-      </c>
-      <c r="I2">
-        <v>100</v>
-      </c>
-      <c r="J2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE6E911-31A5-440C-882A-670D99BCCC80}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2">
-        <v>450</v>
-      </c>
-      <c r="C2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="H2">
-        <v>9</v>
-      </c>
-      <c r="I2">
-        <v>100</v>
-      </c>
-      <c r="J2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D908F63-2316-4814-8934-7E6571A2EA9A}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,7 +865,7 @@
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1119,11 +890,8 @@
       <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
@@ -1147,9 +915,6 @@
       </c>
       <c r="H2" t="s">
         <v>29</v>
-      </c>
-      <c r="I2" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1158,7 +923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3114FEA7-B434-48B1-B4F6-7B4F3BE8673D}">
   <dimension ref="A1:S17"/>
   <sheetViews>
@@ -2502,8 +2267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DBB80D-3005-41F8-86F4-7517B0EFE4BC}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Callables missing from AR TCs.Updated them.
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/AR.xlsx
+++ b/templates/AutomationOrg/AR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B188BF4A-80C9-48CE-BF5B-F39554CADD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3258A391-D5BF-4D67-96EA-8404B4323D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,10 @@
     <sheet name="PickPackShip" sheetId="13" r:id="rId9"/>
     <sheet name="CreateInvoice" sheetId="18" r:id="rId10"/>
     <sheet name="CashReceipt" sheetId="21" r:id="rId11"/>
-    <sheet name="CashReceipt_ForeignCurr" sheetId="22" r:id="rId12"/>
-    <sheet name="ARATO" sheetId="25" r:id="rId13"/>
+    <sheet name="CRATO_HomeCurrency" sheetId="28" r:id="rId12"/>
+    <sheet name="CRATO_ForeignCurrency" sheetId="29" r:id="rId13"/>
+    <sheet name="CashReceipt_ForeignCurr" sheetId="22" r:id="rId14"/>
+    <sheet name="ARATO" sheetId="25" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="104">
   <si>
     <t>API Mode</t>
   </si>
@@ -310,6 +312,54 @@
   </si>
   <si>
     <t>Automation5501-5 (Misc)</t>
+  </si>
+  <si>
+    <t>ComapnyID</t>
+  </si>
+  <si>
+    <t>aBb5f0000004JfX</t>
+  </si>
+  <si>
+    <t>BankAccountID</t>
+  </si>
+  <si>
+    <t>aBT5f000000wmhn</t>
+  </si>
+  <si>
+    <t>Check Payment</t>
+  </si>
+  <si>
+    <t>Transaction Currency</t>
+  </si>
+  <si>
+    <t>a8S5f0000004MBb</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>TransactionAmountMaintCurr</t>
+  </si>
+  <si>
+    <t>HomeCurrtoMaintCurrRate</t>
+  </si>
+  <si>
+    <t>TransactionCurrtoHomeRate</t>
+  </si>
+  <si>
+    <t>Not Yet Processed</t>
+  </si>
+  <si>
+    <t>DiscountTakenMaint Curr</t>
+  </si>
+  <si>
+    <t>CompanyID</t>
+  </si>
+  <si>
+    <t>aBT5f000000wmm0</t>
+  </si>
+  <si>
+    <t>a8S5f0000004NwM</t>
   </si>
 </sst>
 </file>
@@ -370,12 +420,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -774,73 +825,86 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C10D85-D20E-4C13-9DFC-4F2EB5FB623F}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2">
         <v>450</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
       </c>
       <c r="D2">
         <v>100</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>38</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>450</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -851,11 +915,211 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2BC7194-6154-49CA-A8FF-099750D7B793}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2">
+        <v>450</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="L2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE6E911-31A5-440C-882A-670D99BCCC80}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2">
+        <v>450</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="L2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D908F63-2316-4814-8934-7E6571A2EA9A}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,7 +1187,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3114FEA7-B434-48B1-B4F6-7B4F3BE8673D}">
   <dimension ref="A1:S17"/>
   <sheetViews>
@@ -2267,8 +2531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DBB80D-3005-41F8-86F4-7517B0EFE4BC}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated AR TCs and Test Plan
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/AR.xlsx
+++ b/templates/AutomationOrg/AR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3258A391-D5BF-4D67-96EA-8404B4323D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0506DC-2327-410F-A1F2-B8B48EEC277B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-495" yWindow="75" windowWidth="20430" windowHeight="7875" tabRatio="761" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="103">
   <si>
     <t>API Mode</t>
   </si>
@@ -312,9 +312,6 @@
   </si>
   <si>
     <t>Automation5501-5 (Misc)</t>
-  </si>
-  <si>
-    <t>ComapnyID</t>
   </si>
   <si>
     <t>aBb5f0000004JfX</t>
@@ -828,7 +825,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H2"/>
+      <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +846,7 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>25</v>
@@ -861,7 +858,7 @@
         <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="G1" t="s">
         <v>39</v>
@@ -881,7 +878,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2">
         <v>450</v>
@@ -893,7 +890,7 @@
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>40</v>
@@ -919,7 +916,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,13 +929,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
         <v>39</v>
@@ -947,19 +944,19 @@
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K1" t="s">
         <v>26</v>
@@ -970,22 +967,22 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2">
         <v>450</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -994,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J2">
         <v>9</v>
@@ -1016,7 +1013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE6E911-31A5-440C-882A-670D99BCCC80}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -1034,13 +1031,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
         <v>39</v>
@@ -1049,19 +1046,19 @@
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K1" t="s">
         <v>26</v>
@@ -1072,22 +1069,22 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2">
         <v>450</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>78</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1096,7 +1093,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J2">
         <v>9</v>
@@ -1116,20 +1113,20 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D908F63-2316-4814-8934-7E6571A2EA9A}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1143,19 +1140,22 @@
         <v>26</v>
       </c>
       <c r="E1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
@@ -1168,16 +1168,19 @@
       <c r="D2">
         <v>100</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>41</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>450</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2239,7 +2242,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2532,7 +2535,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated ARATO TC and renamed some SO TCs
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/AR.xlsx
+++ b/templates/AutomationOrg/AR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0506DC-2327-410F-A1F2-B8B48EEC277B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB59C586-F820-490B-8F7D-548308BA1561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-495" yWindow="75" windowWidth="20430" windowHeight="7875" tabRatio="761" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21795" yWindow="1365" windowWidth="27270" windowHeight="10890" tabRatio="761" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="100">
   <si>
     <t>API Mode</t>
   </si>
@@ -203,9 +203,6 @@
     <t>Debit Amount</t>
   </si>
   <si>
-    <t>Account</t>
-  </si>
-  <si>
     <t>Posting Type</t>
   </si>
   <si>
@@ -233,21 +230,9 @@
     <t>ExpectedGLTXNCount</t>
   </si>
   <si>
-    <t>a5B41000000PRNXEA4</t>
-  </si>
-  <si>
     <t>Invoice</t>
   </si>
   <si>
-    <t>a9h4100000005tC</t>
-  </si>
-  <si>
-    <t>a9g410000004LBs</t>
-  </si>
-  <si>
-    <t>a9S41000000Gnq3</t>
-  </si>
-  <si>
     <t>Red Widgets</t>
   </si>
   <si>
@@ -269,15 +254,9 @@
     <t>Credit Memo</t>
   </si>
   <si>
-    <t>a9S41000000GntC</t>
-  </si>
-  <si>
     <t>Unapplied Cash</t>
   </si>
   <si>
-    <t>a5B410000004My9EAE</t>
-  </si>
-  <si>
     <t>Pending</t>
   </si>
   <si>
@@ -357,13 +336,25 @@
   </si>
   <si>
     <t>a8S5f0000004NwM</t>
+  </si>
+  <si>
+    <t>GLAccount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  aBE5f000000kKQk</t>
+  </si>
+  <si>
+    <t>aBE5f000000kKS5</t>
+  </si>
+  <si>
+    <t>aBd5f000000oYg0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,6 +386,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -738,7 +735,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -846,7 +843,7 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>25</v>
@@ -858,7 +855,7 @@
         <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G1" t="s">
         <v>39</v>
@@ -878,7 +875,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C2">
         <v>450</v>
@@ -890,7 +887,7 @@
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>40</v>
@@ -929,13 +926,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
         <v>39</v>
@@ -944,19 +941,19 @@
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="K1" t="s">
         <v>26</v>
@@ -967,31 +964,31 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B2">
         <v>450</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="F2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="J2">
         <v>9</v>
@@ -1031,13 +1028,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
         <v>39</v>
@@ -1046,19 +1043,19 @@
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="K1" t="s">
         <v>26</v>
@@ -1069,31 +1066,31 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B2">
         <v>450</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="F2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="J2">
         <v>9</v>
@@ -1115,7 +1112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D908F63-2316-4814-8934-7E6571A2EA9A}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -1140,7 +1137,7 @@
         <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
         <v>39</v>
@@ -1157,7 +1154,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B2">
         <v>450</v>
@@ -1169,10 +1166,10 @@
         <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
         <v>41</v>
@@ -1194,11 +1191,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3114FEA7-B434-48B1-B4F6-7B4F3BE8673D}">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1229,48 +1244,48 @@
         <v>50</v>
       </c>
       <c r="J1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" t="s">
         <v>51</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>52</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>53</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>54</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>55</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>56</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>58</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>59</v>
       </c>
-      <c r="S1" t="s">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
-      </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -1285,48 +1300,48 @@
         <v>500</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="K2">
         <v>651</v>
       </c>
       <c r="L2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2">
+        <v>500</v>
+      </c>
+      <c r="R2">
+        <v>500</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
         <v>66</v>
       </c>
-      <c r="M2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N2" t="s">
-        <v>68</v>
-      </c>
-      <c r="O2" t="s">
-        <v>69</v>
-      </c>
-      <c r="P2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q2">
-        <v>500</v>
-      </c>
-      <c r="R2">
-        <v>500</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" t="s">
-        <v>71</v>
-      </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -1341,48 +1356,48 @@
         <v>500</v>
       </c>
       <c r="J3" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="K3">
         <v>601</v>
       </c>
       <c r="L3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3">
+        <v>500</v>
+      </c>
+      <c r="R3">
+        <v>500</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
         <v>67</v>
       </c>
-      <c r="N3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O3" t="s">
-        <v>69</v>
-      </c>
-      <c r="P3" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q3">
-        <v>500</v>
-      </c>
-      <c r="R3">
-        <v>500</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" t="s">
-        <v>72</v>
-      </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -1397,25 +1412,25 @@
         <v>500</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="K4">
         <v>611</v>
       </c>
       <c r="L4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="Q4">
         <v>-500</v>
@@ -1428,17 +1443,17 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>61</v>
+      <c r="A5" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -1453,25 +1468,25 @@
         <v>500</v>
       </c>
       <c r="J5" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="K5">
         <v>613</v>
       </c>
       <c r="L5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="Q5">
         <v>-500</v>
@@ -1484,17 +1499,17 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>75</v>
+      <c r="A6" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -1509,25 +1524,25 @@
         <v>500</v>
       </c>
       <c r="J6" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="K6">
         <v>651</v>
       </c>
       <c r="L6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="Q6">
         <v>50</v>
@@ -1540,17 +1555,17 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>75</v>
+      <c r="A7" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -1565,25 +1580,25 @@
         <v>500</v>
       </c>
       <c r="J7" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="K7">
         <v>601</v>
       </c>
       <c r="L7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="Q7">
         <v>50</v>
@@ -1596,17 +1611,17 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>75</v>
+      <c r="A8" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -1621,25 +1636,25 @@
         <v>500</v>
       </c>
       <c r="J8" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="K8">
         <v>611</v>
       </c>
       <c r="L8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="Q8">
         <v>-50</v>
@@ -1652,17 +1667,17 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>75</v>
+      <c r="A9" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -1677,25 +1692,25 @@
         <v>500</v>
       </c>
       <c r="J9" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="K9">
         <v>613</v>
       </c>
       <c r="L9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P9" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="Q9">
         <v>-50</v>
@@ -1708,17 +1723,17 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>61</v>
+      <c r="A10" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -1733,25 +1748,25 @@
         <v>500</v>
       </c>
       <c r="J10" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="K10">
         <v>651</v>
       </c>
       <c r="L10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O10" t="s">
+        <v>64</v>
+      </c>
+      <c r="P10" t="s">
         <v>69</v>
-      </c>
-      <c r="P10" t="s">
-        <v>76</v>
       </c>
       <c r="Q10">
         <v>500</v>
@@ -1764,17 +1779,17 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>61</v>
+      <c r="A11" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -1789,25 +1804,25 @@
         <v>500</v>
       </c>
       <c r="J11" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="K11">
         <v>601</v>
       </c>
       <c r="L11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O11" t="s">
+        <v>64</v>
+      </c>
+      <c r="P11" t="s">
         <v>69</v>
-      </c>
-      <c r="P11" t="s">
-        <v>76</v>
       </c>
       <c r="Q11">
         <v>500</v>
@@ -1820,17 +1835,17 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>61</v>
+      <c r="A12" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -1845,25 +1860,25 @@
         <v>500</v>
       </c>
       <c r="J12" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="K12">
         <v>611</v>
       </c>
       <c r="L12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O12" t="s">
+        <v>64</v>
+      </c>
+      <c r="P12" t="s">
         <v>69</v>
-      </c>
-      <c r="P12" t="s">
-        <v>76</v>
       </c>
       <c r="Q12">
         <v>-500</v>
@@ -1876,17 +1891,17 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>61</v>
+      <c r="A13" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -1901,25 +1916,25 @@
         <v>500</v>
       </c>
       <c r="J13" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="K13">
         <v>613</v>
       </c>
       <c r="L13" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O13" t="s">
+        <v>64</v>
+      </c>
+      <c r="P13" t="s">
         <v>69</v>
-      </c>
-      <c r="P13" t="s">
-        <v>76</v>
       </c>
       <c r="Q13">
         <v>-500</v>
@@ -1932,17 +1947,17 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>75</v>
+      <c r="A14" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -1957,25 +1972,25 @@
         <v>500</v>
       </c>
       <c r="J14" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="K14">
         <v>651</v>
       </c>
       <c r="L14" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O14" t="s">
+        <v>64</v>
+      </c>
+      <c r="P14" t="s">
         <v>69</v>
-      </c>
-      <c r="P14" t="s">
-        <v>76</v>
       </c>
       <c r="Q14">
         <v>50</v>
@@ -1988,17 +2003,17 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>75</v>
+      <c r="A15" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -2013,25 +2028,25 @@
         <v>500</v>
       </c>
       <c r="J15" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="K15">
         <v>601</v>
       </c>
       <c r="L15" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O15" t="s">
+        <v>64</v>
+      </c>
+      <c r="P15" t="s">
         <v>69</v>
-      </c>
-      <c r="P15" t="s">
-        <v>76</v>
       </c>
       <c r="Q15">
         <v>50</v>
@@ -2044,17 +2059,17 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>75</v>
+      <c r="A16" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -2069,25 +2084,25 @@
         <v>500</v>
       </c>
       <c r="J16" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="K16">
         <v>611</v>
       </c>
       <c r="L16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N16" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O16" t="s">
+        <v>64</v>
+      </c>
+      <c r="P16" t="s">
         <v>69</v>
-      </c>
-      <c r="P16" t="s">
-        <v>76</v>
       </c>
       <c r="Q16">
         <v>-50</v>
@@ -2100,17 +2115,17 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>75</v>
+      <c r="A17" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -2125,25 +2140,25 @@
         <v>500</v>
       </c>
       <c r="J17" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="K17">
         <v>613</v>
       </c>
       <c r="L17" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="O17" t="s">
+        <v>64</v>
+      </c>
+      <c r="P17" t="s">
         <v>69</v>
-      </c>
-      <c r="P17" t="s">
-        <v>76</v>
       </c>
       <c r="Q17">
         <v>-50</v>
@@ -2156,7 +2171,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2196,7 +2213,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -2283,7 +2300,7 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
@@ -2330,7 +2347,7 @@
         <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -2377,7 +2394,7 @@
         <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -2424,7 +2441,7 @@
         <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -2471,7 +2488,7 @@
         <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I5">
         <v>2</v>
@@ -2509,7 +2526,7 @@
         <v>37</v>
       </c>
       <c r="H6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I6">
         <v>3</v>
@@ -2576,7 +2593,7 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
@@ -2623,7 +2640,7 @@
         <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -2670,7 +2687,7 @@
         <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -2717,7 +2734,7 @@
         <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -2764,7 +2781,7 @@
         <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I5">
         <v>2</v>
@@ -2802,7 +2819,7 @@
         <v>37</v>
       </c>
       <c r="H6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I6">
         <v>3</v>
@@ -2882,7 +2899,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -2919,7 +2936,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Added new TCs for Duplicate SO number, Avalara Tax retained TC...
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/AR.xlsx
+++ b/templates/AutomationOrg/AR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB59C586-F820-490B-8F7D-548308BA1561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E95AB7B-0897-45B7-8E2E-B7C2EDC57FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21795" yWindow="1365" windowWidth="27270" windowHeight="10890" tabRatio="761" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="100">
   <si>
     <t>API Mode</t>
   </si>
@@ -1189,984 +1189,1036 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3114FEA7-B434-48B1-B4F6-7B4F3BE8673D}">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A17"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>96</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>51</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>52</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>53</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>54</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>55</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>57</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>58</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>99</v>
       </c>
-      <c r="D2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>500</v>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="H2">
-        <v>500</v>
-      </c>
-      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>500</v>
+      </c>
+      <c r="K2" t="s">
         <v>97</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>651</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>61</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>62</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>63</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>64</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>65</v>
       </c>
-      <c r="Q2">
-        <v>500</v>
-      </c>
       <c r="R2">
         <v>500</v>
       </c>
       <c r="S2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>99</v>
       </c>
-      <c r="D3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>500</v>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="H3">
-        <v>500</v>
-      </c>
-      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>500</v>
+      </c>
+      <c r="K3" t="s">
         <v>97</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>601</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>61</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>62</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>63</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>64</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>65</v>
       </c>
-      <c r="Q3">
-        <v>500</v>
-      </c>
       <c r="R3">
         <v>500</v>
       </c>
       <c r="S3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>67</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>99</v>
       </c>
-      <c r="D4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>500</v>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>500</v>
-      </c>
-      <c r="J4" t="s">
+        <v>500</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>500</v>
+      </c>
+      <c r="K4" t="s">
         <v>98</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>611</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>61</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>62</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>63</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>64</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>65</v>
-      </c>
-      <c r="Q4">
-        <v>-500</v>
       </c>
       <c r="R4">
         <v>-500</v>
       </c>
       <c r="S4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+        <v>-500</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>68</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>99</v>
       </c>
-      <c r="D5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>500</v>
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>500</v>
-      </c>
-      <c r="J5" t="s">
+        <v>500</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>500</v>
+      </c>
+      <c r="K5" t="s">
         <v>98</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>613</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>61</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>62</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>63</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>64</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>65</v>
-      </c>
-      <c r="Q5">
-        <v>-500</v>
       </c>
       <c r="R5">
         <v>-500</v>
       </c>
       <c r="S5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+        <v>-500</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>60</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>99</v>
       </c>
-      <c r="D6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6">
+      <c r="E6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <v>50</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>10</v>
       </c>
-      <c r="H6">
-        <v>500</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="I6">
+        <v>500</v>
+      </c>
+      <c r="K6" t="s">
         <v>97</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>651</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>61</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>62</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>63</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>64</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>65</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>50</v>
       </c>
-      <c r="R6">
-        <v>500</v>
-      </c>
       <c r="S6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>66</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>99</v>
       </c>
-      <c r="D7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7">
+      <c r="E7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7">
         <v>50</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>10</v>
       </c>
-      <c r="H7">
-        <v>500</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="I7">
+        <v>500</v>
+      </c>
+      <c r="K7" t="s">
         <v>97</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>601</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>61</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>62</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>63</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>64</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>65</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>50</v>
       </c>
-      <c r="R7">
-        <v>500</v>
-      </c>
       <c r="S7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>67</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>99</v>
       </c>
-      <c r="D8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8">
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8">
         <v>50</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>10</v>
       </c>
-      <c r="I8">
-        <v>500</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="J8">
+        <v>500</v>
+      </c>
+      <c r="K8" t="s">
         <v>98</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>611</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>61</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>62</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>63</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>64</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>65</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>-50</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>-500</v>
       </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="T8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>68</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>99</v>
       </c>
-      <c r="D9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9">
+      <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9">
         <v>50</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>10</v>
       </c>
-      <c r="I9">
-        <v>500</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="J9">
+        <v>500</v>
+      </c>
+      <c r="K9" t="s">
         <v>98</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>613</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>61</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>62</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>63</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>64</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>65</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>-50</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>-500</v>
       </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="T9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>60</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>99</v>
       </c>
-      <c r="D10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>500</v>
+      <c r="E10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="H10">
-        <v>500</v>
-      </c>
-      <c r="J10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>500</v>
+      </c>
+      <c r="K10" t="s">
         <v>97</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>651</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>61</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>62</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>63</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>64</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>69</v>
       </c>
-      <c r="Q10">
-        <v>500</v>
-      </c>
       <c r="R10">
         <v>500</v>
       </c>
       <c r="S10">
+        <v>500</v>
+      </c>
+      <c r="T10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>66</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>99</v>
       </c>
-      <c r="D11" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>500</v>
+      <c r="E11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="H11">
-        <v>500</v>
-      </c>
-      <c r="J11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>500</v>
+      </c>
+      <c r="K11" t="s">
         <v>97</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>601</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>61</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>62</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>63</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>64</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>69</v>
       </c>
-      <c r="Q11">
-        <v>500</v>
-      </c>
       <c r="R11">
         <v>500</v>
       </c>
       <c r="S11">
+        <v>500</v>
+      </c>
+      <c r="T11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>67</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>99</v>
       </c>
-      <c r="D12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>500</v>
+      <c r="E12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>500</v>
-      </c>
-      <c r="J12" t="s">
+        <v>500</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>500</v>
+      </c>
+      <c r="K12" t="s">
         <v>98</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>611</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>61</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>62</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>63</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>64</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>69</v>
-      </c>
-      <c r="Q12">
-        <v>-500</v>
       </c>
       <c r="R12">
         <v>-500</v>
       </c>
       <c r="S12">
+        <v>-500</v>
+      </c>
+      <c r="T12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>68</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>99</v>
       </c>
-      <c r="D13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>500</v>
+      <c r="E13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>500</v>
-      </c>
-      <c r="J13" t="s">
+        <v>500</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>500</v>
+      </c>
+      <c r="K13" t="s">
         <v>98</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>613</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>61</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>62</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>63</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>64</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>69</v>
-      </c>
-      <c r="Q13">
-        <v>-500</v>
       </c>
       <c r="R13">
         <v>-500</v>
       </c>
       <c r="S13">
+        <v>-500</v>
+      </c>
+      <c r="T13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>60</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>99</v>
       </c>
-      <c r="D14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14">
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14">
         <v>50</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>10</v>
       </c>
-      <c r="H14">
-        <v>500</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="I14">
+        <v>500</v>
+      </c>
+      <c r="K14" t="s">
         <v>97</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>651</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>61</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>62</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>63</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>64</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>69</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>50</v>
       </c>
-      <c r="R14">
-        <v>500</v>
-      </c>
       <c r="S14">
+        <v>500</v>
+      </c>
+      <c r="T14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>66</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>99</v>
       </c>
-      <c r="D15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15">
+      <c r="E15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15">
         <v>50</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>10</v>
       </c>
-      <c r="H15">
-        <v>500</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="I15">
+        <v>500</v>
+      </c>
+      <c r="K15" t="s">
         <v>97</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>601</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>61</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>62</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>63</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>64</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>69</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>50</v>
       </c>
-      <c r="R15">
-        <v>500</v>
-      </c>
       <c r="S15">
+        <v>500</v>
+      </c>
+      <c r="T15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>67</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>99</v>
       </c>
-      <c r="D16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16">
+      <c r="E16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16">
         <v>50</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>10</v>
       </c>
-      <c r="I16">
-        <v>500</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="J16">
+        <v>500</v>
+      </c>
+      <c r="K16" t="s">
         <v>98</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>611</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>61</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>62</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>63</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>64</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>69</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>-50</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>-500</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>68</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>99</v>
       </c>
-      <c r="D17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17">
+      <c r="E17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17">
         <v>50</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>10</v>
       </c>
-      <c r="I17">
-        <v>500</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="J17">
+        <v>500</v>
+      </c>
+      <c r="K17" t="s">
         <v>98</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>613</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>61</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>62</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>63</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>64</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>69</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>-50</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>-500</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated AR TC (added SOCustCmpnyNo field on CRATO)
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/AR.xlsx
+++ b/templates/AutomationOrg/AR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E95AB7B-0897-45B7-8E2E-B7C2EDC57FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F689AE37-DB57-4E7D-94AB-EA47BCBDA6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" tabRatio="761" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="2205" windowWidth="15375" windowHeight="7875" tabRatio="761" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="103">
   <si>
     <t>API Mode</t>
   </si>
@@ -348,6 +348,15 @@
   </si>
   <si>
     <t>aBd5f000000oYg0</t>
+  </si>
+  <si>
+    <t>CustomerCompany</t>
+  </si>
+  <si>
+    <t>aCc5f0000000C0S</t>
+  </si>
+  <si>
+    <t>aCc5f0000000BKH</t>
   </si>
 </sst>
 </file>
@@ -910,10 +919,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2BC7194-6154-49CA-A8FF-099750D7B793}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +933,7 @@
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -961,8 +970,11 @@
       <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -998,6 +1010,9 @@
       </c>
       <c r="L2" t="s">
         <v>38</v>
+      </c>
+      <c r="M2" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1008,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE6E911-31A5-440C-882A-670D99BCCC80}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1041,7 @@
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -1063,8 +1078,11 @@
       <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -1100,6 +1118,9 @@
       </c>
       <c r="L2" t="s">
         <v>41</v>
+      </c>
+      <c r="M2" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1191,7 +1212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3114FEA7-B434-48B1-B4F6-7B4F3BE8673D}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>